<commit_message>
more styling of output
</commit_message>
<xml_diff>
--- a/data/Workday_Data_Sample.xlsx
+++ b/data/Workday_Data_Sample.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{C36379A1-4CA6-41F7-B0D6-B3C611C05CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13484FB7-B1AC-4114-B7FC-F8208726CA9C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0F06FC5F-71E8-454C-AFF3-E71EB29B266F}"/>
+    <workbookView minimized="1" xWindow="12080" yWindow="1630" windowWidth="2370" windowHeight="560" xr2:uid="{0F06FC5F-71E8-454C-AFF3-E71EB29B266F}"/>
   </bookViews>
   <sheets>
     <sheet name="Workday Data 05092025" sheetId="1" r:id="rId1"/>
@@ -15113,8 +15113,8 @@
   <dimension ref="A1:I2483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A1112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1121" sqref="G1121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>